<commit_message>
Completar codigo de los modelso
</commit_message>
<xml_diff>
--- a/ExtraClase/Documencation-EMNA/EMNA-Documentacion.xlsx
+++ b/ExtraClase/Documencation-EMNA/EMNA-Documentacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arias Ramirez\OneDrive\Escritorio\U\2024-2\IS2\ExtraClase\Documencation-EMNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381D62FC-E9D9-48D8-8DDB-051DB140963F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC12EA-F2EE-48AF-80CA-162B481C45A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="994">
   <si>
     <t>Trade off de QA</t>
   </si>
@@ -3955,6 +3955,9 @@
   </si>
   <si>
     <t xml:space="preserve">Resultado de la solicutud, representando los datos en un formato adecuado. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repositorio </t>
   </si>
 </sst>
 </file>
@@ -4570,7 +4573,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -4880,14 +4883,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4897,6 +4915,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4910,52 +4931,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4976,26 +4955,50 @@
     <xf numFmtId="0" fontId="13" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5017,6 +5020,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5084,23 +5105,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -9842,9 +9848,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -9856,168 +9864,173 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="19"/>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="115" t="s">
         <v>369</v>
       </c>
-      <c r="C1" s="113"/>
+      <c r="C1" s="115"/>
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="37" t="s">
         <v>370</v>
       </c>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="116" t="s">
         <v>367</v>
       </c>
-      <c r="C2" s="114"/>
+      <c r="C2" s="116"/>
       <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="64.5" customHeight="1">
       <c r="A3" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="116" t="s">
         <v>368</v>
       </c>
-      <c r="C3" s="114"/>
+      <c r="C3" s="116"/>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="66.75" customHeight="1">
       <c r="A4" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="116" t="s">
         <v>378</v>
       </c>
-      <c r="C4" s="114"/>
+      <c r="C4" s="116"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="7"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="187" t="s">
+        <v>993</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="111" t="s">
         <v>892</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B8" s="93" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="91" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="91" t="s">
         <v>427</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B9" s="109" t="s">
         <v>894</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="90" t="s">
-        <v>351</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="90" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="90" t="s">
+        <v>352</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="90" t="s">
         <v>353</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B12" s="110" t="s">
         <v>904</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="92" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="92" t="s">
         <v>157</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B13" s="21" t="s">
         <v>905</v>
       </c>
-      <c r="C12" s="112"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="90" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="110" t="s">
-        <v>906</v>
-      </c>
+      <c r="C13" s="112"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="90" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="109" t="s">
-        <v>895</v>
+        <v>0</v>
+      </c>
+      <c r="B14" s="110" t="s">
+        <v>906</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="109" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="110" t="s">
+      <c r="B16" s="110" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="92" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="92" t="s">
         <v>428</v>
       </c>
-      <c r="B16" s="110" t="s">
+      <c r="B17" s="110" t="s">
         <v>861</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="90" t="s">
-        <v>429</v>
-      </c>
-      <c r="B17" s="109" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="90" t="s">
+        <v>429</v>
+      </c>
+      <c r="B18" s="109" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="90" t="s">
         <v>430</v>
       </c>
-      <c r="B18" s="110" t="s">
+      <c r="B19" s="110" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="92" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="92" t="s">
         <v>592</v>
       </c>
-      <c r="B19" s="110" t="s">
+      <c r="B20" s="110" t="s">
         <v>898</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="90" t="s">
-        <v>593</v>
-      </c>
-      <c r="B20" s="110" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="90" t="s">
+        <v>593</v>
+      </c>
+      <c r="B21" s="110" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="90" t="s">
         <v>657</v>
       </c>
-      <c r="B21" s="109" t="s">
+      <c r="B22" s="109" t="s">
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="B22" s="110" t="s">
+    <row r="23" spans="1:2">
+      <c r="B23" s="110" t="s">
         <v>901</v>
       </c>
     </row>
@@ -10029,27 +10042,28 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A13" location="'Trade off '!A1" display="Trade off de QA" xr:uid="{DFE46B2E-658A-485B-9FB6-398B7CA63E1C}"/>
-    <hyperlink ref="A14" location="'Mapa Empatia'!A1" display="Mapa de Empatia " xr:uid="{E0A6560C-961F-4860-8ADD-F07043445D12}"/>
-    <hyperlink ref="A15" location="Caracterizacion!A1" display="Caractetizacion " xr:uid="{ED93357A-4E55-4391-83A1-412B54BBAC90}"/>
-    <hyperlink ref="A9" location="RestriccionesNegocio!A1" display="Restricciones de negocio " xr:uid="{0C18D978-5861-41CF-BD36-498C54063DDD}"/>
-    <hyperlink ref="A10" location="'FuncionalidadesCriticas '!A1" display="Funcionalidades criticas " xr:uid="{6B62D9FA-8469-430A-80EB-5235B982B64B}"/>
-    <hyperlink ref="A11" location="RestriccionesTecnicas!A1" display="Restricciones Tecnicas " xr:uid="{E9BB16F9-6A9E-4871-AA6E-22D047375EE8}"/>
-    <hyperlink ref="A17" location="AlternativaSolucionSelecc!A1" display="Alternativa de Solucion  Seleccionada" xr:uid="{AA444825-5E3A-4194-9D21-A73A8AAD0A74}"/>
-    <hyperlink ref="A18" location="TacticasEstrategias!A1" display="Tacticas Estrategias" xr:uid="{39CB7AEA-71C0-4D59-86DB-D19AE6DA3AA3}"/>
-    <hyperlink ref="A20" location="Elecciones!A1" display="Elecciones  " xr:uid="{3B377A59-6A47-4FFC-924C-34F4E5A642B4}"/>
-    <hyperlink ref="A21" location="'Provedores Componentes'!A1" display="Provedores Componentes" xr:uid="{3B24E8FF-73DC-4B5B-A04A-E708E817B7EF}"/>
-    <hyperlink ref="B15" location="'Diagrama de componentes '!A1" display="Diagrama de componentes " xr:uid="{4D28DDDE-FA0F-4FB7-BBCA-53ADDEA1FA71}"/>
-    <hyperlink ref="B16" location="'Diagrama de paquetes '!A1" display="Diagrama de paquetes " xr:uid="{82047B9E-CBE2-41F3-A60A-CD1457D7E16F}"/>
-    <hyperlink ref="B22" location="'Img-Arquetipo de solucion '!A1" display="Arquetipo de solucion " xr:uid="{EFBDB4D2-1410-431E-AEE0-A6DDCE4693DB}"/>
-    <hyperlink ref="B19" location="'Img-Arquetipo de solucion '!A1" display="Diagrama de comunicaciones " xr:uid="{B1B81DC1-A086-42B5-8CE3-82825931D90E}"/>
-    <hyperlink ref="B11" location="'Img-Modelo de dominio '!A1" display="Modelo de dominio " xr:uid="{2092BDA8-9C1C-41DB-86A7-C285D5A7246F}"/>
-    <hyperlink ref="B13" location="'Img-Modelo de entidad relacion '!A1" display="Modelo de entidad relacion " xr:uid="{88A84F18-A83E-46D9-875F-AD7BF1ACC0C4}"/>
-    <hyperlink ref="B20" location="'Img-Diagrama de actividades '!A1" display="Diagrama de actividades " xr:uid="{256C662F-55E5-40F9-8E58-002110C950B2}"/>
-    <hyperlink ref="B18" location="'Diagrama de secuencias '!A1" display="Diagrama de secuencias " xr:uid="{CF8057B7-5FB4-40F7-8779-C5DDBB682750}"/>
+    <hyperlink ref="A14" location="'Trade off '!A1" display="Trade off de QA" xr:uid="{DFE46B2E-658A-485B-9FB6-398B7CA63E1C}"/>
+    <hyperlink ref="A15" location="'Mapa Empatia'!A1" display="Mapa de Empatia " xr:uid="{E0A6560C-961F-4860-8ADD-F07043445D12}"/>
+    <hyperlink ref="A16" location="Caracterizacion!A1" display="Caractetizacion " xr:uid="{ED93357A-4E55-4391-83A1-412B54BBAC90}"/>
+    <hyperlink ref="A10" location="RestriccionesNegocio!A1" display="Restricciones de negocio " xr:uid="{0C18D978-5861-41CF-BD36-498C54063DDD}"/>
+    <hyperlink ref="A11" location="'FuncionalidadesCriticas '!A1" display="Funcionalidades criticas " xr:uid="{6B62D9FA-8469-430A-80EB-5235B982B64B}"/>
+    <hyperlink ref="A12" location="RestriccionesTecnicas!A1" display="Restricciones Tecnicas " xr:uid="{E9BB16F9-6A9E-4871-AA6E-22D047375EE8}"/>
+    <hyperlink ref="A18" location="AlternativaSolucionSelecc!A1" display="Alternativa de Solucion  Seleccionada" xr:uid="{AA444825-5E3A-4194-9D21-A73A8AAD0A74}"/>
+    <hyperlink ref="A19" location="TacticasEstrategias!A1" display="Tacticas Estrategias" xr:uid="{39CB7AEA-71C0-4D59-86DB-D19AE6DA3AA3}"/>
+    <hyperlink ref="A21" location="Elecciones!A1" display="Elecciones  " xr:uid="{3B377A59-6A47-4FFC-924C-34F4E5A642B4}"/>
+    <hyperlink ref="A22" location="'Provedores Componentes'!A1" display="Provedores Componentes" xr:uid="{3B24E8FF-73DC-4B5B-A04A-E708E817B7EF}"/>
+    <hyperlink ref="B16" location="'Diagrama de componentes '!A1" display="Diagrama de componentes " xr:uid="{4D28DDDE-FA0F-4FB7-BBCA-53ADDEA1FA71}"/>
+    <hyperlink ref="B17" location="'Diagrama de paquetes '!A1" display="Diagrama de paquetes " xr:uid="{82047B9E-CBE2-41F3-A60A-CD1457D7E16F}"/>
+    <hyperlink ref="B23" location="'Img-Arquetipo de solucion '!A1" display="Arquetipo de solucion " xr:uid="{EFBDB4D2-1410-431E-AEE0-A6DDCE4693DB}"/>
+    <hyperlink ref="B20" location="'Img-Arquetipo de solucion '!A1" display="Diagrama de comunicaciones " xr:uid="{B1B81DC1-A086-42B5-8CE3-82825931D90E}"/>
+    <hyperlink ref="B12" location="'Img-Modelo de dominio '!A1" display="Modelo de dominio " xr:uid="{2092BDA8-9C1C-41DB-86A7-C285D5A7246F}"/>
+    <hyperlink ref="B14" location="'Img-Modelo de entidad relacion '!A1" display="Modelo de entidad relacion " xr:uid="{88A84F18-A83E-46D9-875F-AD7BF1ACC0C4}"/>
+    <hyperlink ref="B21" location="'Img-Diagrama de actividades '!A1" display="Diagrama de actividades " xr:uid="{256C662F-55E5-40F9-8E58-002110C950B2}"/>
+    <hyperlink ref="B19" location="'Diagrama de secuencias '!A1" display="Diagrama de secuencias " xr:uid="{CF8057B7-5FB4-40F7-8779-C5DDBB682750}"/>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{33230388-71F1-4C76-ADCC-E3DCAEF9BC67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10074,58 +10088,58 @@
       <c r="A1" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="124" t="s">
         <v>941</v>
       </c>
-      <c r="C1" s="115"/>
+      <c r="C1" s="124"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="102" t="s">
         <v>862</v>
       </c>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="149" t="s">
         <v>873</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="102" t="s">
         <v>863</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="149" t="s">
         <v>884</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
     </row>
     <row r="4" spans="1:6" ht="42.75" customHeight="1">
       <c r="A4" s="102" t="s">
         <v>864</v>
       </c>
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="149" t="s">
         <v>913</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149"/>
+      <c r="F4" s="149"/>
     </row>
     <row r="5" spans="1:6" ht="31.5" customHeight="1">
       <c r="A5" s="102" t="s">
         <v>865</v>
       </c>
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="149" t="s">
         <v>914</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="102" t="s">
@@ -10140,320 +10154,320 @@
       <c r="D6" s="102" t="s">
         <v>867</v>
       </c>
-      <c r="E6" s="126" t="s">
+      <c r="E6" s="150" t="s">
         <v>868</v>
       </c>
-      <c r="F6" s="126"/>
+      <c r="F6" s="150"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="127" t="s">
+      <c r="A7" s="143" t="s">
         <v>873</v>
       </c>
-      <c r="B7" s="127" t="s">
+      <c r="B7" s="143" t="s">
         <v>878</v>
       </c>
       <c r="C7" s="103" t="s">
         <v>879</v>
       </c>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127" t="s">
+      <c r="D7" s="143"/>
+      <c r="E7" s="143" t="s">
         <v>913</v>
       </c>
-      <c r="F7" s="127"/>
+      <c r="F7" s="143"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="127"/>
-      <c r="B8" s="127"/>
+      <c r="A8" s="143"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="103" t="s">
         <v>880</v>
       </c>
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
+      <c r="D8" s="143"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="143"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="127"/>
-      <c r="B9" s="127"/>
+      <c r="A9" s="143"/>
+      <c r="B9" s="143"/>
       <c r="C9" s="103" t="s">
         <v>882</v>
       </c>
-      <c r="D9" s="127"/>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127"/>
+      <c r="D9" s="143"/>
+      <c r="E9" s="143"/>
+      <c r="F9" s="143"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="143" t="s">
         <v>879</v>
       </c>
-      <c r="B10" s="127" t="s">
+      <c r="B10" s="143" t="s">
         <v>877</v>
       </c>
-      <c r="C10" s="127"/>
+      <c r="C10" s="143"/>
       <c r="D10" s="103" t="s">
         <v>883</v>
       </c>
-      <c r="E10" s="127" t="s">
+      <c r="E10" s="143" t="s">
         <v>910</v>
       </c>
-      <c r="F10" s="127"/>
+      <c r="F10" s="143"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="127"/>
-      <c r="B11" s="127"/>
-      <c r="C11" s="127"/>
+      <c r="A11" s="143"/>
+      <c r="B11" s="143"/>
+      <c r="C11" s="143"/>
       <c r="D11" s="103" t="s">
         <v>880</v>
       </c>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
+      <c r="E11" s="143"/>
+      <c r="F11" s="143"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="127"/>
-      <c r="B12" s="127"/>
-      <c r="C12" s="127"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="143"/>
+      <c r="C12" s="143"/>
       <c r="D12" s="103" t="s">
         <v>882</v>
       </c>
-      <c r="E12" s="127"/>
-      <c r="F12" s="127"/>
+      <c r="E12" s="143"/>
+      <c r="F12" s="143"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="127" t="s">
+      <c r="A13" s="143" t="s">
         <v>880</v>
       </c>
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="143" t="s">
         <v>877</v>
       </c>
-      <c r="C13" s="136" t="s">
+      <c r="C13" s="144" t="s">
         <v>879</v>
       </c>
       <c r="D13" s="103" t="s">
         <v>883</v>
       </c>
-      <c r="E13" s="139" t="s">
+      <c r="E13" s="131" t="s">
         <v>911</v>
       </c>
-      <c r="F13" s="140"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="127"/>
-      <c r="B14" s="127"/>
-      <c r="C14" s="137"/>
+      <c r="A14" s="143"/>
+      <c r="B14" s="143"/>
+      <c r="C14" s="145"/>
       <c r="D14" s="104" t="s">
         <v>874</v>
       </c>
-      <c r="E14" s="141"/>
-      <c r="F14" s="142"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="134"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="127"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="137"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="143"/>
+      <c r="C15" s="145"/>
       <c r="D15" s="104" t="s">
         <v>875</v>
       </c>
-      <c r="E15" s="141"/>
-      <c r="F15" s="142"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="134"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="127"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="138"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="143"/>
+      <c r="C16" s="146"/>
       <c r="D16" s="104" t="s">
         <v>876</v>
       </c>
-      <c r="E16" s="143"/>
-      <c r="F16" s="144"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="136"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="127" t="s">
+      <c r="A17" s="143" t="s">
         <v>881</v>
       </c>
-      <c r="B17" s="127" t="s">
+      <c r="B17" s="143" t="s">
         <v>877</v>
       </c>
-      <c r="C17" s="136" t="s">
+      <c r="C17" s="144" t="s">
         <v>879</v>
       </c>
       <c r="D17" s="103" t="s">
         <v>883</v>
       </c>
-      <c r="E17" s="128" t="s">
+      <c r="E17" s="137" t="s">
         <v>912</v>
       </c>
-      <c r="F17" s="129"/>
+      <c r="F17" s="138"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="127"/>
-      <c r="B18" s="127"/>
-      <c r="C18" s="137"/>
+      <c r="A18" s="143"/>
+      <c r="B18" s="143"/>
+      <c r="C18" s="145"/>
       <c r="D18" s="104" t="s">
         <v>874</v>
       </c>
-      <c r="E18" s="134"/>
-      <c r="F18" s="135"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="140"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="127"/>
-      <c r="B19" s="127"/>
-      <c r="C19" s="137"/>
+      <c r="A19" s="143"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="145"/>
       <c r="D19" s="104" t="s">
         <v>875</v>
       </c>
-      <c r="E19" s="134"/>
-      <c r="F19" s="135"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="140"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="127"/>
-      <c r="B20" s="127"/>
-      <c r="C20" s="138"/>
+      <c r="A20" s="143"/>
+      <c r="B20" s="143"/>
+      <c r="C20" s="146"/>
       <c r="D20" s="104" t="s">
         <v>876</v>
       </c>
-      <c r="E20" s="130"/>
-      <c r="F20" s="131"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="142"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="122" t="s">
+      <c r="A21" s="128" t="s">
         <v>874</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="128" t="s">
         <v>878</v>
       </c>
       <c r="C21" s="103" t="s">
         <v>879</v>
       </c>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="128" t="s">
         <v>883</v>
       </c>
-      <c r="E21" s="128" t="s">
+      <c r="E21" s="137" t="s">
         <v>908</v>
       </c>
-      <c r="F21" s="129"/>
+      <c r="F21" s="138"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="124"/>
-      <c r="B22" s="124"/>
+      <c r="A22" s="129"/>
+      <c r="B22" s="129"/>
       <c r="C22" s="103" t="s">
         <v>880</v>
       </c>
-      <c r="D22" s="124"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="135"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="140"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="123"/>
-      <c r="B23" s="123"/>
+      <c r="A23" s="130"/>
+      <c r="B23" s="130"/>
       <c r="C23" s="103" t="s">
         <v>882</v>
       </c>
-      <c r="D23" s="123"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="131"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="141"/>
+      <c r="F23" s="142"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="122" t="s">
+      <c r="A24" s="128" t="s">
         <v>875</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="128" t="s">
         <v>878</v>
       </c>
       <c r="C24" s="103" t="s">
         <v>879</v>
       </c>
-      <c r="D24" s="122" t="s">
+      <c r="D24" s="128" t="s">
         <v>883</v>
       </c>
-      <c r="E24" s="128" t="s">
+      <c r="E24" s="137" t="s">
         <v>907</v>
       </c>
-      <c r="F24" s="129"/>
+      <c r="F24" s="138"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="124"/>
-      <c r="B25" s="124"/>
+      <c r="A25" s="129"/>
+      <c r="B25" s="129"/>
       <c r="C25" s="103" t="s">
         <v>880</v>
       </c>
-      <c r="D25" s="124"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="135"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="140"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="123"/>
-      <c r="B26" s="123"/>
+      <c r="A26" s="130"/>
+      <c r="B26" s="130"/>
       <c r="C26" s="103" t="s">
         <v>882</v>
       </c>
-      <c r="D26" s="123"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="131"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="142"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="122" t="s">
+      <c r="A27" s="128" t="s">
         <v>876</v>
       </c>
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="128" t="s">
         <v>878</v>
       </c>
       <c r="C27" s="103" t="s">
         <v>879</v>
       </c>
-      <c r="D27" s="122" t="s">
+      <c r="D27" s="128" t="s">
         <v>883</v>
       </c>
-      <c r="E27" s="128" t="s">
+      <c r="E27" s="137" t="s">
         <v>909</v>
       </c>
-      <c r="F27" s="129"/>
+      <c r="F27" s="138"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="124"/>
-      <c r="B28" s="124"/>
+      <c r="A28" s="129"/>
+      <c r="B28" s="129"/>
       <c r="C28" s="103" t="s">
         <v>880</v>
       </c>
-      <c r="D28" s="124"/>
-      <c r="E28" s="134"/>
-      <c r="F28" s="135"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="140"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="123"/>
-      <c r="B29" s="123"/>
+      <c r="A29" s="130"/>
+      <c r="B29" s="130"/>
       <c r="C29" s="103" t="s">
         <v>882</v>
       </c>
-      <c r="D29" s="123"/>
-      <c r="E29" s="130"/>
-      <c r="F29" s="131"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="141"/>
+      <c r="F29" s="142"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="122" t="s">
+      <c r="A30" s="128" t="s">
         <v>916</v>
       </c>
-      <c r="B30" s="122" t="s">
+      <c r="B30" s="128" t="s">
         <v>877</v>
       </c>
       <c r="C30" s="104" t="s">
         <v>917</v>
       </c>
-      <c r="D30" s="122" t="s">
+      <c r="D30" s="128" t="s">
         <v>891</v>
       </c>
-      <c r="E30" s="128" t="s">
+      <c r="E30" s="137" t="s">
         <v>910</v>
       </c>
-      <c r="F30" s="129"/>
+      <c r="F30" s="138"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="123"/>
-      <c r="B31" s="123"/>
+      <c r="A31" s="130"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="104" t="s">
         <v>915</v>
       </c>
-      <c r="D31" s="123"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="131"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="141"/>
+      <c r="F31" s="142"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="104" t="s">
@@ -10466,10 +10480,10 @@
       <c r="D32" s="104" t="s">
         <v>891</v>
       </c>
-      <c r="E32" s="132" t="s">
+      <c r="E32" s="147" t="s">
         <v>910</v>
       </c>
-      <c r="F32" s="133"/>
+      <c r="F32" s="148"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="104" t="s">
@@ -10482,55 +10496,71 @@
       <c r="D33" s="104" t="s">
         <v>891</v>
       </c>
-      <c r="E33" s="132" t="s">
+      <c r="E33" s="147" t="s">
         <v>910</v>
       </c>
-      <c r="F33" s="133"/>
+      <c r="F33" s="148"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="122" t="s">
+      <c r="A34" s="128" t="s">
         <v>891</v>
       </c>
-      <c r="B34" s="122" t="s">
+      <c r="B34" s="128" t="s">
         <v>878</v>
       </c>
       <c r="C34" s="104" t="s">
         <v>916</v>
       </c>
-      <c r="D34" s="122"/>
-      <c r="E34" s="128" t="s">
+      <c r="D34" s="128"/>
+      <c r="E34" s="137" t="s">
         <v>918</v>
       </c>
-      <c r="F34" s="129"/>
+      <c r="F34" s="138"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="124"/>
-      <c r="B35" s="124"/>
+      <c r="A35" s="129"/>
+      <c r="B35" s="129"/>
       <c r="C35" s="104" t="s">
         <v>917</v>
       </c>
-      <c r="D35" s="124"/>
-      <c r="E35" s="134"/>
-      <c r="F35" s="135"/>
+      <c r="D35" s="129"/>
+      <c r="E35" s="139"/>
+      <c r="F35" s="140"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="123"/>
-      <c r="B36" s="123"/>
+      <c r="A36" s="130"/>
+      <c r="B36" s="130"/>
       <c r="C36" s="104" t="s">
         <v>915</v>
       </c>
-      <c r="D36" s="123"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="131"/>
+      <c r="D36" s="130"/>
+      <c r="E36" s="141"/>
+      <c r="F36" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E13:F16"/>
-    <mergeCell ref="E17:F20"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="E24:F26"/>
-    <mergeCell ref="E27:F29"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E30:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F36"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="E10:F12"/>
@@ -10547,28 +10577,12 @@
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F36"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E13:F16"/>
+    <mergeCell ref="E17:F20"/>
+    <mergeCell ref="E21:F23"/>
+    <mergeCell ref="E24:F26"/>
+    <mergeCell ref="E27:F29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{32414F91-C2A5-47DD-93EA-9C2CBC6A25AC}"/>
@@ -11542,914 +11556,914 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1">
-      <c r="A3" s="145">
+      <c r="A3" s="151">
         <v>1</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="151" t="s">
         <v>471</v>
       </c>
       <c r="C3" s="73" t="s">
         <v>472</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="145"/>
-      <c r="B4" s="145"/>
+      <c r="A4" s="151"/>
+      <c r="B4" s="151"/>
       <c r="C4" s="73" t="s">
         <v>473</v>
       </c>
-      <c r="D4" s="145"/>
-      <c r="E4" s="145"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1">
-      <c r="A5" s="145">
+      <c r="A5" s="151">
         <v>2</v>
       </c>
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="151" t="s">
         <v>476</v>
       </c>
       <c r="C5" s="73" t="s">
         <v>477</v>
       </c>
-      <c r="D5" s="145" t="s">
+      <c r="D5" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E5" s="145" t="s">
+      <c r="E5" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="145"/>
-      <c r="B6" s="145"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="151"/>
       <c r="C6" s="73" t="s">
         <v>478</v>
       </c>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1">
-      <c r="A7" s="145">
+      <c r="A7" s="151">
         <v>3</v>
       </c>
-      <c r="B7" s="145" t="s">
+      <c r="B7" s="151" t="s">
         <v>532</v>
       </c>
       <c r="C7" s="73" t="s">
         <v>479</v>
       </c>
-      <c r="D7" s="145" t="s">
+      <c r="D7" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E7" s="145" t="s">
+      <c r="E7" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="145"/>
-      <c r="B8" s="145"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="151"/>
       <c r="C8" s="73" t="s">
         <v>480</v>
       </c>
-      <c r="D8" s="145"/>
-      <c r="E8" s="145"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="151"/>
     </row>
     <row r="9" spans="1:5" ht="60" customHeight="1">
-      <c r="A9" s="145">
+      <c r="A9" s="151">
         <v>4</v>
       </c>
-      <c r="B9" s="145" t="s">
+      <c r="B9" s="151" t="s">
         <v>481</v>
       </c>
       <c r="C9" s="73" t="s">
         <v>482</v>
       </c>
-      <c r="D9" s="145" t="s">
+      <c r="D9" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E9" s="145" t="s">
+      <c r="E9" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="145"/>
-      <c r="B10" s="145"/>
+      <c r="A10" s="151"/>
+      <c r="B10" s="151"/>
       <c r="C10" s="73" t="s">
         <v>483</v>
       </c>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
     </row>
     <row r="11" spans="1:5" ht="45" customHeight="1">
-      <c r="A11" s="145">
+      <c r="A11" s="151">
         <v>5</v>
       </c>
-      <c r="B11" s="145" t="s">
+      <c r="B11" s="151" t="s">
         <v>538</v>
       </c>
       <c r="C11" s="73" t="s">
         <v>485</v>
       </c>
-      <c r="D11" s="145" t="s">
+      <c r="D11" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E11" s="145" t="s">
+      <c r="E11" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="145"/>
-      <c r="B12" s="145"/>
+      <c r="A12" s="151"/>
+      <c r="B12" s="151"/>
       <c r="C12" s="73" t="s">
         <v>486</v>
       </c>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1">
-      <c r="A13" s="145">
+      <c r="A13" s="151">
         <v>6</v>
       </c>
-      <c r="B13" s="145" t="s">
+      <c r="B13" s="151" t="s">
         <v>487</v>
       </c>
       <c r="C13" s="73" t="s">
         <v>488</v>
       </c>
-      <c r="D13" s="145" t="s">
+      <c r="D13" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E13" s="145" t="s">
+      <c r="E13" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="145"/>
-      <c r="B14" s="145"/>
+      <c r="A14" s="151"/>
+      <c r="B14" s="151"/>
       <c r="C14" s="73" t="s">
         <v>489</v>
       </c>
-      <c r="D14" s="145"/>
-      <c r="E14" s="145"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
     </row>
     <row r="15" spans="1:5" ht="45" customHeight="1">
-      <c r="A15" s="145">
+      <c r="A15" s="151">
         <v>7</v>
       </c>
-      <c r="B15" s="145" t="s">
+      <c r="B15" s="151" t="s">
         <v>490</v>
       </c>
       <c r="C15" s="73" t="s">
         <v>491</v>
       </c>
-      <c r="D15" s="145" t="s">
+      <c r="D15" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E15" s="145" t="s">
+      <c r="E15" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="145"/>
-      <c r="B16" s="145"/>
+      <c r="A16" s="151"/>
+      <c r="B16" s="151"/>
       <c r="C16" s="73" t="s">
         <v>492</v>
       </c>
-      <c r="D16" s="145"/>
-      <c r="E16" s="145"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
     </row>
     <row r="17" spans="1:5" ht="45" customHeight="1">
-      <c r="A17" s="145">
+      <c r="A17" s="151">
         <v>8</v>
       </c>
-      <c r="B17" s="145" t="s">
+      <c r="B17" s="151" t="s">
         <v>493</v>
       </c>
       <c r="C17" s="73" t="s">
         <v>494</v>
       </c>
-      <c r="D17" s="145" t="s">
+      <c r="D17" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E17" s="145" t="s">
+      <c r="E17" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="145"/>
-      <c r="B18" s="145"/>
+      <c r="A18" s="151"/>
+      <c r="B18" s="151"/>
       <c r="C18" s="73" t="s">
         <v>495</v>
       </c>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1">
-      <c r="A19" s="145">
+      <c r="A19" s="151">
         <v>9</v>
       </c>
-      <c r="B19" s="145" t="s">
+      <c r="B19" s="151" t="s">
         <v>496</v>
       </c>
       <c r="C19" s="73" t="s">
         <v>497</v>
       </c>
-      <c r="D19" s="145" t="s">
+      <c r="D19" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E19" s="145" t="s">
+      <c r="E19" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30">
-      <c r="A20" s="145"/>
-      <c r="B20" s="145"/>
+      <c r="A20" s="151"/>
+      <c r="B20" s="151"/>
       <c r="C20" s="73" t="s">
         <v>498</v>
       </c>
-      <c r="D20" s="145"/>
-      <c r="E20" s="145"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1">
-      <c r="A21" s="145">
+      <c r="A21" s="151">
         <v>10</v>
       </c>
-      <c r="B21" s="145" t="s">
+      <c r="B21" s="151" t="s">
         <v>499</v>
       </c>
       <c r="C21" s="73" t="s">
         <v>500</v>
       </c>
-      <c r="D21" s="145" t="s">
+      <c r="D21" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E21" s="145" t="s">
+      <c r="E21" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="145"/>
-      <c r="B22" s="145"/>
+      <c r="A22" s="151"/>
+      <c r="B22" s="151"/>
       <c r="C22" s="73" t="s">
         <v>501</v>
       </c>
-      <c r="D22" s="145"/>
-      <c r="E22" s="145"/>
+      <c r="D22" s="151"/>
+      <c r="E22" s="151"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="145">
+      <c r="A23" s="151">
         <v>11</v>
       </c>
-      <c r="B23" s="145" t="s">
+      <c r="B23" s="151" t="s">
         <v>502</v>
       </c>
       <c r="C23" s="73" t="s">
         <v>503</v>
       </c>
-      <c r="D23" s="145" t="s">
+      <c r="D23" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E23" s="145" t="s">
+      <c r="E23" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30">
-      <c r="A24" s="145"/>
-      <c r="B24" s="145"/>
+      <c r="A24" s="151"/>
+      <c r="B24" s="151"/>
       <c r="C24" s="73" t="s">
         <v>504</v>
       </c>
-      <c r="D24" s="145"/>
-      <c r="E24" s="145"/>
+      <c r="D24" s="151"/>
+      <c r="E24" s="151"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1">
-      <c r="A25" s="145">
+      <c r="A25" s="151">
         <v>12</v>
       </c>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="151" t="s">
         <v>505</v>
       </c>
       <c r="C25" s="73" t="s">
         <v>506</v>
       </c>
-      <c r="D25" s="145" t="s">
+      <c r="D25" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E25" s="145" t="s">
+      <c r="E25" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30">
-      <c r="A26" s="145"/>
-      <c r="B26" s="145"/>
+      <c r="A26" s="151"/>
+      <c r="B26" s="151"/>
       <c r="C26" s="73" t="s">
         <v>507</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="E26" s="145"/>
+      <c r="D26" s="151"/>
+      <c r="E26" s="151"/>
     </row>
     <row r="27" spans="1:5" ht="45" customHeight="1">
-      <c r="A27" s="145">
+      <c r="A27" s="151">
         <v>13</v>
       </c>
-      <c r="B27" s="145" t="s">
+      <c r="B27" s="151" t="s">
         <v>508</v>
       </c>
       <c r="C27" s="73" t="s">
         <v>509</v>
       </c>
-      <c r="D27" s="145" t="s">
+      <c r="D27" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E27" s="145" t="s">
+      <c r="E27" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="145"/>
-      <c r="B28" s="145"/>
+      <c r="A28" s="151"/>
+      <c r="B28" s="151"/>
       <c r="C28" s="73" t="s">
         <v>510</v>
       </c>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
+      <c r="D28" s="151"/>
+      <c r="E28" s="151"/>
     </row>
     <row r="29" spans="1:5" ht="45" customHeight="1">
-      <c r="A29" s="145">
+      <c r="A29" s="151">
         <v>14</v>
       </c>
-      <c r="B29" s="145" t="s">
+      <c r="B29" s="151" t="s">
         <v>511</v>
       </c>
       <c r="C29" s="73" t="s">
         <v>512</v>
       </c>
-      <c r="D29" s="145" t="s">
+      <c r="D29" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E29" s="145" t="s">
+      <c r="E29" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30">
-      <c r="A30" s="145"/>
-      <c r="B30" s="145"/>
+      <c r="A30" s="151"/>
+      <c r="B30" s="151"/>
       <c r="C30" s="73" t="s">
         <v>513</v>
       </c>
-      <c r="D30" s="145"/>
-      <c r="E30" s="145"/>
+      <c r="D30" s="151"/>
+      <c r="E30" s="151"/>
     </row>
     <row r="31" spans="1:5" ht="45" customHeight="1">
-      <c r="A31" s="145">
+      <c r="A31" s="151">
         <v>15</v>
       </c>
-      <c r="B31" s="145" t="s">
+      <c r="B31" s="151" t="s">
         <v>514</v>
       </c>
       <c r="C31" s="73" t="s">
         <v>515</v>
       </c>
-      <c r="D31" s="145" t="s">
+      <c r="D31" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E31" s="145" t="s">
+      <c r="E31" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="145"/>
-      <c r="B32" s="145"/>
+      <c r="A32" s="151"/>
+      <c r="B32" s="151"/>
       <c r="C32" s="73" t="s">
         <v>516</v>
       </c>
-      <c r="D32" s="145"/>
-      <c r="E32" s="145"/>
+      <c r="D32" s="151"/>
+      <c r="E32" s="151"/>
     </row>
     <row r="33" spans="1:5" ht="45" customHeight="1">
-      <c r="A33" s="145">
+      <c r="A33" s="151">
         <v>16</v>
       </c>
-      <c r="B33" s="145" t="s">
+      <c r="B33" s="151" t="s">
         <v>517</v>
       </c>
       <c r="C33" s="73" t="s">
         <v>518</v>
       </c>
-      <c r="D33" s="145" t="s">
+      <c r="D33" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E33" s="145" t="s">
+      <c r="E33" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30">
-      <c r="A34" s="145"/>
-      <c r="B34" s="145"/>
+      <c r="A34" s="151"/>
+      <c r="B34" s="151"/>
       <c r="C34" s="73" t="s">
         <v>519</v>
       </c>
-      <c r="D34" s="145"/>
-      <c r="E34" s="145"/>
+      <c r="D34" s="151"/>
+      <c r="E34" s="151"/>
     </row>
     <row r="35" spans="1:5" ht="30" customHeight="1">
-      <c r="A35" s="145">
+      <c r="A35" s="151">
         <v>17</v>
       </c>
-      <c r="B35" s="145" t="s">
+      <c r="B35" s="151" t="s">
         <v>520</v>
       </c>
       <c r="C35" s="73" t="s">
         <v>521</v>
       </c>
-      <c r="D35" s="145" t="s">
+      <c r="D35" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E35" s="145" t="s">
+      <c r="E35" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30">
-      <c r="A36" s="145"/>
-      <c r="B36" s="145"/>
+      <c r="A36" s="151"/>
+      <c r="B36" s="151"/>
       <c r="C36" s="73" t="s">
         <v>522</v>
       </c>
-      <c r="D36" s="145"/>
-      <c r="E36" s="145"/>
+      <c r="D36" s="151"/>
+      <c r="E36" s="151"/>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1">
-      <c r="A37" s="145">
+      <c r="A37" s="151">
         <v>18</v>
       </c>
-      <c r="B37" s="145" t="s">
+      <c r="B37" s="151" t="s">
         <v>523</v>
       </c>
       <c r="C37" s="73" t="s">
         <v>524</v>
       </c>
-      <c r="D37" s="145" t="s">
+      <c r="D37" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E37" s="145" t="s">
+      <c r="E37" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30">
-      <c r="A38" s="145"/>
-      <c r="B38" s="145"/>
+      <c r="A38" s="151"/>
+      <c r="B38" s="151"/>
       <c r="C38" s="73" t="s">
         <v>525</v>
       </c>
-      <c r="D38" s="145"/>
-      <c r="E38" s="145"/>
+      <c r="D38" s="151"/>
+      <c r="E38" s="151"/>
     </row>
     <row r="39" spans="1:5" ht="45" customHeight="1">
-      <c r="A39" s="145">
+      <c r="A39" s="151">
         <v>19</v>
       </c>
-      <c r="B39" s="145" t="s">
+      <c r="B39" s="151" t="s">
         <v>526</v>
       </c>
       <c r="C39" s="73" t="s">
         <v>527</v>
       </c>
-      <c r="D39" s="145" t="s">
+      <c r="D39" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E39" s="145" t="s">
+      <c r="E39" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="45">
-      <c r="A40" s="145"/>
-      <c r="B40" s="145"/>
+      <c r="A40" s="151"/>
+      <c r="B40" s="151"/>
       <c r="C40" s="73" t="s">
         <v>528</v>
       </c>
-      <c r="D40" s="145"/>
-      <c r="E40" s="145"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="151"/>
     </row>
     <row r="41" spans="1:5" ht="45" customHeight="1">
-      <c r="A41" s="145">
+      <c r="A41" s="151">
         <v>20</v>
       </c>
-      <c r="B41" s="145" t="s">
+      <c r="B41" s="151" t="s">
         <v>529</v>
       </c>
       <c r="C41" s="73" t="s">
         <v>530</v>
       </c>
-      <c r="D41" s="145" t="s">
+      <c r="D41" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E41" s="145" t="s">
+      <c r="E41" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30">
-      <c r="A42" s="145"/>
-      <c r="B42" s="145"/>
+      <c r="A42" s="151"/>
+      <c r="B42" s="151"/>
       <c r="C42" s="73" t="s">
         <v>531</v>
       </c>
-      <c r="D42" s="145"/>
-      <c r="E42" s="145"/>
+      <c r="D42" s="151"/>
+      <c r="E42" s="151"/>
     </row>
     <row r="43" spans="1:5" ht="45" customHeight="1">
-      <c r="A43" s="145">
+      <c r="A43" s="151">
         <v>21</v>
       </c>
-      <c r="B43" s="145" t="s">
+      <c r="B43" s="151" t="s">
         <v>546</v>
       </c>
       <c r="C43" s="73" t="s">
         <v>547</v>
       </c>
-      <c r="D43" s="145" t="s">
+      <c r="D43" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E43" s="145" t="s">
+      <c r="E43" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" customHeight="1">
-      <c r="A44" s="145"/>
-      <c r="B44" s="145"/>
+      <c r="A44" s="151"/>
+      <c r="B44" s="151"/>
       <c r="C44" s="73" t="s">
         <v>548</v>
       </c>
-      <c r="D44" s="145"/>
-      <c r="E44" s="145"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="151"/>
     </row>
     <row r="45" spans="1:5" ht="30" customHeight="1">
-      <c r="A45" s="145">
+      <c r="A45" s="151">
         <v>22</v>
       </c>
-      <c r="B45" s="145" t="s">
+      <c r="B45" s="151" t="s">
         <v>549</v>
       </c>
       <c r="C45" s="73" t="s">
         <v>550</v>
       </c>
-      <c r="D45" s="145" t="s">
+      <c r="D45" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E45" s="145" t="s">
+      <c r="E45" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1">
-      <c r="A46" s="145"/>
-      <c r="B46" s="145"/>
+      <c r="A46" s="151"/>
+      <c r="B46" s="151"/>
       <c r="C46" s="73" t="s">
         <v>551</v>
       </c>
-      <c r="D46" s="145"/>
-      <c r="E46" s="145"/>
+      <c r="D46" s="151"/>
+      <c r="E46" s="151"/>
     </row>
     <row r="47" spans="1:5" ht="45" customHeight="1">
-      <c r="A47" s="145">
+      <c r="A47" s="151">
         <v>23</v>
       </c>
-      <c r="B47" s="145" t="s">
+      <c r="B47" s="151" t="s">
         <v>552</v>
       </c>
       <c r="C47" s="73" t="s">
         <v>553</v>
       </c>
-      <c r="D47" s="145" t="s">
+      <c r="D47" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E47" s="145" t="s">
+      <c r="E47" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="30" customHeight="1">
-      <c r="A48" s="145"/>
-      <c r="B48" s="145"/>
+      <c r="A48" s="151"/>
+      <c r="B48" s="151"/>
       <c r="C48" s="73" t="s">
         <v>554</v>
       </c>
-      <c r="D48" s="145"/>
-      <c r="E48" s="145"/>
+      <c r="D48" s="151"/>
+      <c r="E48" s="151"/>
     </row>
     <row r="49" spans="1:5" ht="45" customHeight="1">
-      <c r="A49" s="145">
+      <c r="A49" s="151">
         <v>24</v>
       </c>
-      <c r="B49" s="145" t="s">
+      <c r="B49" s="151" t="s">
         <v>555</v>
       </c>
       <c r="C49" s="73" t="s">
         <v>556</v>
       </c>
-      <c r="D49" s="145" t="s">
+      <c r="D49" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E49" s="145" t="s">
+      <c r="E49" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" customHeight="1">
-      <c r="A50" s="145"/>
-      <c r="B50" s="145"/>
+      <c r="A50" s="151"/>
+      <c r="B50" s="151"/>
       <c r="C50" s="73" t="s">
         <v>557</v>
       </c>
-      <c r="D50" s="145"/>
-      <c r="E50" s="145"/>
+      <c r="D50" s="151"/>
+      <c r="E50" s="151"/>
     </row>
     <row r="51" spans="1:5" ht="45" customHeight="1">
-      <c r="A51" s="145">
+      <c r="A51" s="151">
         <v>25</v>
       </c>
-      <c r="B51" s="145" t="s">
+      <c r="B51" s="151" t="s">
         <v>558</v>
       </c>
       <c r="C51" s="73" t="s">
         <v>559</v>
       </c>
-      <c r="D51" s="145" t="s">
+      <c r="D51" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E51" s="145" t="s">
+      <c r="E51" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" customHeight="1">
-      <c r="A52" s="145"/>
-      <c r="B52" s="145"/>
+      <c r="A52" s="151"/>
+      <c r="B52" s="151"/>
       <c r="C52" s="73" t="s">
         <v>560</v>
       </c>
-      <c r="D52" s="145"/>
-      <c r="E52" s="145"/>
+      <c r="D52" s="151"/>
+      <c r="E52" s="151"/>
     </row>
     <row r="53" spans="1:5" ht="30" customHeight="1">
-      <c r="A53" s="145">
+      <c r="A53" s="151">
         <v>26</v>
       </c>
-      <c r="B53" s="145" t="s">
+      <c r="B53" s="151" t="s">
         <v>561</v>
       </c>
       <c r="C53" s="73" t="s">
         <v>562</v>
       </c>
-      <c r="D53" s="145" t="s">
+      <c r="D53" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E53" s="145" t="s">
+      <c r="E53" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="30" customHeight="1">
-      <c r="A54" s="145"/>
-      <c r="B54" s="145"/>
+      <c r="A54" s="151"/>
+      <c r="B54" s="151"/>
       <c r="C54" s="73" t="s">
         <v>563</v>
       </c>
-      <c r="D54" s="145"/>
-      <c r="E54" s="145"/>
+      <c r="D54" s="151"/>
+      <c r="E54" s="151"/>
     </row>
     <row r="55" spans="1:5" ht="30" customHeight="1">
-      <c r="A55" s="145">
+      <c r="A55" s="151">
         <v>27</v>
       </c>
-      <c r="B55" s="145" t="s">
+      <c r="B55" s="151" t="s">
         <v>564</v>
       </c>
       <c r="C55" s="73" t="s">
         <v>565</v>
       </c>
-      <c r="D55" s="145" t="s">
+      <c r="D55" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E55" s="145" t="s">
+      <c r="E55" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" customHeight="1">
-      <c r="A56" s="145"/>
-      <c r="B56" s="145"/>
+      <c r="A56" s="151"/>
+      <c r="B56" s="151"/>
       <c r="C56" s="73" t="s">
         <v>566</v>
       </c>
-      <c r="D56" s="145"/>
-      <c r="E56" s="145"/>
+      <c r="D56" s="151"/>
+      <c r="E56" s="151"/>
     </row>
     <row r="57" spans="1:5" ht="45" customHeight="1">
-      <c r="A57" s="145">
+      <c r="A57" s="151">
         <v>28</v>
       </c>
-      <c r="B57" s="145" t="s">
+      <c r="B57" s="151" t="s">
         <v>567</v>
       </c>
       <c r="C57" s="73" t="s">
         <v>568</v>
       </c>
-      <c r="D57" s="145" t="s">
+      <c r="D57" s="151" t="s">
         <v>570</v>
       </c>
-      <c r="E57" s="145" t="s">
+      <c r="E57" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" customHeight="1">
-      <c r="A58" s="145"/>
-      <c r="B58" s="145"/>
+      <c r="A58" s="151"/>
+      <c r="B58" s="151"/>
       <c r="C58" s="73" t="s">
         <v>569</v>
       </c>
-      <c r="D58" s="145"/>
-      <c r="E58" s="145"/>
+      <c r="D58" s="151"/>
+      <c r="E58" s="151"/>
     </row>
     <row r="59" spans="1:5" ht="30" customHeight="1">
-      <c r="A59" s="145">
+      <c r="A59" s="151">
         <v>29</v>
       </c>
-      <c r="B59" s="145" t="s">
+      <c r="B59" s="151" t="s">
         <v>571</v>
       </c>
       <c r="C59" s="73" t="s">
         <v>572</v>
       </c>
-      <c r="D59" s="145" t="s">
+      <c r="D59" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E59" s="145" t="s">
+      <c r="E59" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" customHeight="1">
-      <c r="A60" s="145"/>
-      <c r="B60" s="145"/>
+      <c r="A60" s="151"/>
+      <c r="B60" s="151"/>
       <c r="C60" s="73" t="s">
         <v>573</v>
       </c>
-      <c r="D60" s="145"/>
-      <c r="E60" s="145"/>
+      <c r="D60" s="151"/>
+      <c r="E60" s="151"/>
     </row>
     <row r="61" spans="1:5" ht="30">
-      <c r="A61" s="145">
+      <c r="A61" s="151">
         <v>30</v>
       </c>
-      <c r="B61" s="145" t="s">
+      <c r="B61" s="151" t="s">
         <v>574</v>
       </c>
       <c r="C61" s="73" t="s">
         <v>575</v>
       </c>
-      <c r="D61" s="145" t="s">
+      <c r="D61" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E61" s="145" t="s">
+      <c r="E61" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="60" customHeight="1">
-      <c r="A62" s="145"/>
-      <c r="B62" s="145"/>
+      <c r="A62" s="151"/>
+      <c r="B62" s="151"/>
       <c r="C62" s="73" t="s">
         <v>576</v>
       </c>
-      <c r="D62" s="145"/>
-      <c r="E62" s="145"/>
+      <c r="D62" s="151"/>
+      <c r="E62" s="151"/>
     </row>
     <row r="63" spans="1:5" ht="30">
-      <c r="A63" s="145">
+      <c r="A63" s="151">
         <v>31</v>
       </c>
-      <c r="B63" s="145" t="s">
+      <c r="B63" s="151" t="s">
         <v>577</v>
       </c>
       <c r="C63" s="73" t="s">
         <v>578</v>
       </c>
-      <c r="D63" s="145" t="s">
+      <c r="D63" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E63" s="145" t="s">
+      <c r="E63" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="45" customHeight="1">
-      <c r="A64" s="145"/>
-      <c r="B64" s="145"/>
+      <c r="A64" s="151"/>
+      <c r="B64" s="151"/>
       <c r="C64" s="73" t="s">
         <v>579</v>
       </c>
-      <c r="D64" s="145"/>
-      <c r="E64" s="145"/>
+      <c r="D64" s="151"/>
+      <c r="E64" s="151"/>
     </row>
     <row r="65" spans="1:5" ht="45" customHeight="1">
-      <c r="A65" s="145">
+      <c r="A65" s="151">
         <v>32</v>
       </c>
-      <c r="B65" s="145" t="s">
+      <c r="B65" s="151" t="s">
         <v>580</v>
       </c>
       <c r="C65" s="73" t="s">
         <v>581</v>
       </c>
-      <c r="D65" s="145" t="s">
+      <c r="D65" s="151" t="s">
         <v>484</v>
       </c>
-      <c r="E65" s="145" t="s">
+      <c r="E65" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" customHeight="1">
-      <c r="A66" s="145"/>
-      <c r="B66" s="145"/>
+      <c r="A66" s="151"/>
+      <c r="B66" s="151"/>
       <c r="C66" s="73" t="s">
         <v>582</v>
       </c>
-      <c r="D66" s="145"/>
-      <c r="E66" s="145"/>
+      <c r="D66" s="151"/>
+      <c r="E66" s="151"/>
     </row>
     <row r="67" spans="1:5" ht="30" customHeight="1">
-      <c r="A67" s="145">
+      <c r="A67" s="151">
         <v>33</v>
       </c>
-      <c r="B67" s="145" t="s">
+      <c r="B67" s="151" t="s">
         <v>583</v>
       </c>
       <c r="C67" s="73" t="s">
         <v>584</v>
       </c>
-      <c r="D67" s="145" t="s">
+      <c r="D67" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E67" s="145" t="s">
+      <c r="E67" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="45" customHeight="1">
-      <c r="A68" s="145"/>
-      <c r="B68" s="145"/>
+      <c r="A68" s="151"/>
+      <c r="B68" s="151"/>
       <c r="C68" s="73" t="s">
         <v>585</v>
       </c>
-      <c r="D68" s="145"/>
-      <c r="E68" s="145"/>
+      <c r="D68" s="151"/>
+      <c r="E68" s="151"/>
     </row>
     <row r="69" spans="1:5" ht="30" customHeight="1">
-      <c r="A69" s="145">
+      <c r="A69" s="151">
         <v>34</v>
       </c>
-      <c r="B69" s="145" t="s">
+      <c r="B69" s="151" t="s">
         <v>586</v>
       </c>
       <c r="C69" s="73" t="s">
         <v>587</v>
       </c>
-      <c r="D69" s="145" t="s">
+      <c r="D69" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E69" s="145" t="s">
+      <c r="E69" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" customHeight="1">
-      <c r="A70" s="145"/>
-      <c r="B70" s="145"/>
+      <c r="A70" s="151"/>
+      <c r="B70" s="151"/>
       <c r="C70" s="73" t="s">
         <v>588</v>
       </c>
-      <c r="D70" s="145"/>
-      <c r="E70" s="145"/>
+      <c r="D70" s="151"/>
+      <c r="E70" s="151"/>
     </row>
     <row r="71" spans="1:5" ht="30" customHeight="1">
-      <c r="A71" s="145">
+      <c r="A71" s="151">
         <v>35</v>
       </c>
-      <c r="B71" s="145" t="s">
+      <c r="B71" s="151" t="s">
         <v>589</v>
       </c>
       <c r="C71" s="73" t="s">
         <v>590</v>
       </c>
-      <c r="D71" s="145" t="s">
+      <c r="D71" s="151" t="s">
         <v>474</v>
       </c>
-      <c r="E71" s="145" t="s">
+      <c r="E71" s="151" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" customHeight="1">
-      <c r="A72" s="145"/>
-      <c r="B72" s="145"/>
+      <c r="A72" s="151"/>
+      <c r="B72" s="151"/>
       <c r="C72" s="73" t="s">
         <v>591</v>
       </c>
-      <c r="D72" s="145"/>
-      <c r="E72" s="145"/>
+      <c r="D72" s="151"/>
+      <c r="E72" s="151"/>
     </row>
     <row r="74" spans="1:5" ht="30" customHeight="1"/>
     <row r="76" spans="1:5" ht="30" customHeight="1"/>
@@ -12471,6 +12485,122 @@
     <row r="108" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="140">
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
     <mergeCell ref="A59:A60"/>
     <mergeCell ref="B59:B60"/>
     <mergeCell ref="D59:D60"/>
@@ -12495,122 +12625,6 @@
     <mergeCell ref="E69:E70"/>
     <mergeCell ref="D63:D64"/>
     <mergeCell ref="E63:E64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{39E8F964-FA78-451F-AA99-AC92C3995828}"/>
@@ -13397,13 +13411,13 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="45">
-      <c r="A53" s="146" t="s">
+      <c r="A53" s="159" t="s">
         <v>445</v>
       </c>
-      <c r="B53" s="148" t="s">
+      <c r="B53" s="161" t="s">
         <v>446</v>
       </c>
-      <c r="C53" s="150" t="s">
+      <c r="C53" s="163" t="s">
         <v>447</v>
       </c>
       <c r="D53" s="62">
@@ -13432,9 +13446,9 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="45">
-      <c r="A54" s="147"/>
-      <c r="B54" s="149"/>
-      <c r="C54" s="151"/>
+      <c r="A54" s="160"/>
+      <c r="B54" s="162"/>
+      <c r="C54" s="164"/>
       <c r="D54" s="64">
         <v>2</v>
       </c>
@@ -13689,6 +13703,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:K51"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
@@ -13697,17 +13722,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:K4"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:K51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="C50:C52"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
@@ -14352,112 +14366,112 @@
       <c r="A1" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="182" t="s">
+      <c r="B1" s="118" t="s">
         <v>942</v>
       </c>
-      <c r="C1" s="182"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="113" t="s">
         <v>862</v>
       </c>
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="119" t="s">
         <v>951</v>
       </c>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="183" t="s">
+      <c r="A3" s="113" t="s">
         <v>863</v>
       </c>
-      <c r="B3" s="184"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="184"/>
-      <c r="H3" s="184"/>
-      <c r="I3" s="184"/>
+      <c r="B3" s="119"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="119"/>
     </row>
     <row r="4" spans="1:9" ht="30">
-      <c r="A4" s="183" t="s">
+      <c r="A4" s="113" t="s">
         <v>864</v>
       </c>
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="119" t="s">
         <v>952</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" ht="30">
-      <c r="A5" s="183" t="s">
+      <c r="A5" s="113" t="s">
         <v>865</v>
       </c>
-      <c r="B5" s="184" t="s">
+      <c r="B5" s="119" t="s">
         <v>953</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="185" t="s">
+      <c r="A6" s="117" t="s">
         <v>944</v>
       </c>
-      <c r="B6" s="185" t="s">
+      <c r="B6" s="117" t="s">
         <v>945</v>
       </c>
-      <c r="C6" s="185" t="s">
+      <c r="C6" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="185" t="s">
+      <c r="D6" s="117" t="s">
         <v>946</v>
       </c>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185" t="s">
+      <c r="E6" s="117"/>
+      <c r="F6" s="117" t="s">
         <v>947</v>
       </c>
-      <c r="G6" s="185"/>
-      <c r="H6" s="185" t="s">
+      <c r="G6" s="117"/>
+      <c r="H6" s="117" t="s">
         <v>948</v>
       </c>
-      <c r="I6" s="185" t="s">
+      <c r="I6" s="117" t="s">
         <v>949</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="185"/>
-      <c r="B7" s="185"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="186" t="s">
+      <c r="A7" s="117"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="114" t="s">
         <v>950</v>
       </c>
-      <c r="E7" s="186" t="s">
+      <c r="E7" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="186" t="s">
+      <c r="F7" s="114" t="s">
         <v>950</v>
       </c>
-      <c r="G7" s="183" t="s">
+      <c r="G7" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="185"/>
-      <c r="I7" s="185"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="117"/>
     </row>
     <row r="8" spans="1:9" ht="75">
       <c r="A8" s="85">
@@ -14751,6 +14765,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="B1:C1"/>
@@ -14758,11 +14777,6 @@
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{5CDBEF4A-A5B6-4A59-8E5E-F6AC866A8050}"/>
@@ -16709,74 +16723,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="166" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="167" t="s">
         <v>412</v>
       </c>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="166" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="166" t="s">
         <v>348</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="166"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="12" t="s">
@@ -16910,75 +16924,75 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="166"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="172"/>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="173" t="s">
         <v>314</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="175"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="164" t="s">
+      <c r="B4" s="170" t="s">
         <v>349</v>
       </c>
-      <c r="C4" s="165"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
-      <c r="I4" s="166"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="172"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="164" t="s">
+      <c r="B5" s="170" t="s">
         <v>350</v>
       </c>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="166"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="171"/>
+      <c r="E5" s="171"/>
+      <c r="F5" s="171"/>
+      <c r="G5" s="171"/>
+      <c r="H5" s="171"/>
+      <c r="I5" s="172"/>
       <c r="Q5" s="32"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="168" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="163"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="169"/>
+      <c r="H6" s="169"/>
+      <c r="I6" s="169"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="33" t="s">
@@ -17143,74 +17157,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="170" t="s">
         <v>423</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="166"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="172"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="173" t="s">
         <v>406</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="175"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="166" t="s">
         <v>343</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="166" t="s">
         <v>344</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="166"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="12" t="s">
@@ -17376,74 +17390,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="170" t="s">
         <v>423</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="166"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="172"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="173" t="s">
         <v>407</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="175"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="166" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="166" t="s">
         <v>346</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="166"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9" ht="30">
       <c r="A7" s="12" t="s">
@@ -17609,74 +17623,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="170" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="166"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="172"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="173" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="175"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="166" t="s">
         <v>339</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="166" t="s">
         <v>340</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="166"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="12" t="s">
@@ -17839,74 +17853,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="166"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="172"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="173" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="175"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="166" t="s">
         <v>341</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="166" t="s">
         <v>342</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="166"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9" ht="30">
       <c r="A7" s="12" t="s">
@@ -18069,74 +18083,74 @@
       <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
-      <c r="I2" s="172"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="178"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="174" t="s">
+      <c r="B3" s="180" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="174"/>
-      <c r="H3" s="174"/>
-      <c r="I3" s="174"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="180"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="180"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="173" t="s">
+      <c r="B4" s="179" t="s">
         <v>335</v>
       </c>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="173"/>
+      <c r="C4" s="179"/>
+      <c r="D4" s="179"/>
+      <c r="E4" s="179"/>
+      <c r="F4" s="179"/>
+      <c r="G4" s="179"/>
+      <c r="H4" s="179"/>
+      <c r="I4" s="179"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="176" t="s">
         <v>336</v>
       </c>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="171"/>
-      <c r="F5" s="171"/>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="172"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="177"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="178"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="12" t="s">
@@ -18296,68 +18310,68 @@
       <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="B2" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
-      <c r="I2" s="172"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="178"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="174"/>
-      <c r="H3" s="174"/>
-      <c r="I3" s="174"/>
+      <c r="B3" s="180"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="180"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="180"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="173"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="173"/>
+      <c r="B4" s="179"/>
+      <c r="C4" s="179"/>
+      <c r="D4" s="179"/>
+      <c r="E4" s="179"/>
+      <c r="F4" s="179"/>
+      <c r="G4" s="179"/>
+      <c r="H4" s="179"/>
+      <c r="I4" s="179"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="171"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="171"/>
-      <c r="F5" s="171"/>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="172"/>
+      <c r="B5" s="176"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="177"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="178"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9" ht="30">
       <c r="A7" s="12" t="s">
@@ -18478,74 +18492,74 @@
       <c r="A2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="170" t="s">
         <v>534</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="166"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="172"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="173" t="s">
         <v>271</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="175"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="166" t="s">
         <v>337</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
-      <c r="I4" s="160"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="166" t="s">
         <v>338</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="166"/>
+      <c r="E5" s="166"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
+      <c r="I5" s="166"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="12" t="s">
@@ -18699,10 +18713,10 @@
       <c r="A1" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="181" t="s">
+      <c r="B1" s="120" t="s">
         <v>943</v>
       </c>
-      <c r="C1" s="181"/>
+      <c r="C1" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18752,74 +18766,74 @@
       <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="181"/>
+      <c r="H2" s="181"/>
+      <c r="I2" s="181"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="170" t="s">
+      <c r="B3" s="176" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="171"/>
-      <c r="I3" s="172"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="178"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="171"/>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="172"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="178"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="173" t="s">
+      <c r="B5" s="179" t="s">
         <v>196</v>
       </c>
-      <c r="C5" s="173"/>
-      <c r="D5" s="173"/>
-      <c r="E5" s="173"/>
-      <c r="F5" s="173"/>
-      <c r="G5" s="173"/>
-      <c r="H5" s="173"/>
-      <c r="I5" s="173"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="179"/>
+      <c r="G5" s="179"/>
+      <c r="H5" s="179"/>
+      <c r="I5" s="179"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="12" t="s">
@@ -19040,74 +19054,74 @@
       <c r="A2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="164" t="s">
+      <c r="B3" s="170" t="s">
         <v>374</v>
       </c>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="177"/>
-      <c r="G3" s="177"/>
-      <c r="H3" s="177"/>
-      <c r="I3" s="178"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="184"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="185" t="s">
         <v>197</v>
       </c>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="178"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="184"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="166" t="s">
         <v>373</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="180"/>
-      <c r="E5" s="180"/>
-      <c r="F5" s="180"/>
-      <c r="G5" s="180"/>
-      <c r="H5" s="180"/>
-      <c r="I5" s="180"/>
+      <c r="C5" s="186"/>
+      <c r="D5" s="186"/>
+      <c r="E5" s="186"/>
+      <c r="F5" s="186"/>
+      <c r="G5" s="186"/>
+      <c r="H5" s="186"/>
+      <c r="I5" s="186"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="165" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="159"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="159"/>
-      <c r="E6" s="159"/>
-      <c r="F6" s="159"/>
-      <c r="G6" s="159"/>
-      <c r="H6" s="159"/>
-      <c r="I6" s="159"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="12" t="s">
@@ -20092,58 +20106,58 @@
       <c r="A1" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="124" t="s">
         <v>941</v>
       </c>
-      <c r="C1" s="115"/>
+      <c r="C1" s="124"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="95" t="s">
         <v>862</v>
       </c>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="125" t="s">
         <v>884</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="121"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="127"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="95" t="s">
         <v>863</v>
       </c>
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="125" t="s">
         <v>873</v>
       </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="121"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="127"/>
     </row>
     <row r="4" spans="1:6" ht="32.25" customHeight="1">
       <c r="A4" s="95" t="s">
         <v>864</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="125" t="s">
         <v>939</v>
       </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="121"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="127"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="95" t="s">
         <v>865</v>
       </c>
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="125" t="s">
         <v>940</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="121"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="127"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="95" t="s">
@@ -20178,7 +20192,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="116" t="str">
+      <c r="A8" s="121" t="str">
         <f>$B$7</f>
         <v xml:space="preserve">emna-extraclase </v>
       </c>
@@ -20193,12 +20207,12 @@
         <v>emna-extraclase /emnaMensajesMS</v>
       </c>
       <c r="E8" s="96"/>
-      <c r="F8" s="116" t="s">
+      <c r="F8" s="121" t="s">
         <v>920</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="118"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
       <c r="D9" s="96" t="str">
@@ -20206,10 +20220,10 @@
         <v>emna-extraclase /emnaUsuariosMS</v>
       </c>
       <c r="E9" s="96"/>
-      <c r="F9" s="118"/>
+      <c r="F9" s="123"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="117"/>
+      <c r="A10" s="122"/>
       <c r="B10" s="96"/>
       <c r="C10" s="96"/>
       <c r="D10" s="96" t="str">
@@ -20217,7 +20231,7 @@
         <v>emna-extraclase /emnaSeguridadMS</v>
       </c>
       <c r="E10" s="96"/>
-      <c r="F10" s="117"/>
+      <c r="F10" s="122"/>
     </row>
     <row r="11" spans="1:6" ht="30">
       <c r="A11" s="94" t="str">
@@ -20280,7 +20294,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="116" t="str">
+      <c r="A14" s="121" t="str">
         <f t="shared" si="0"/>
         <v>emna-extraclase /emnaMensajesMS</v>
       </c>
@@ -20299,12 +20313,12 @@
         <f>C13</f>
         <v xml:space="preserve">emna-extraclase /emnaMensajesMS/urls </v>
       </c>
-      <c r="F14" s="116" t="s">
+      <c r="F14" s="121" t="s">
         <v>924</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="117"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="96"/>
       <c r="C15" s="96"/>
       <c r="D15" s="96" t="str">
@@ -20312,7 +20326,7 @@
         <v xml:space="preserve">emna-extraclase /emnaMensajesMS/models </v>
       </c>
       <c r="E15" s="96"/>
-      <c r="F15" s="117"/>
+      <c r="F15" s="122"/>
     </row>
     <row r="16" spans="1:6" ht="30">
       <c r="A16" s="77" t="str">
@@ -20339,7 +20353,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="116" t="str">
+      <c r="A17" s="121" t="str">
         <f t="shared" si="0"/>
         <v>emna-extraclase /emnaMensajesMS</v>
       </c>
@@ -20355,12 +20369,12 @@
         <f>C14</f>
         <v xml:space="preserve">emna-extraclase /emnaMensajesMS/views </v>
       </c>
-      <c r="F17" s="116" t="s">
+      <c r="F17" s="121" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="117"/>
+      <c r="A18" s="122"/>
       <c r="B18" s="96"/>
       <c r="C18" s="96"/>
       <c r="D18" s="96"/>
@@ -20368,7 +20382,7 @@
         <f>C16</f>
         <v xml:space="preserve">emna-extraclase /emnaMensajesMS/serializers </v>
       </c>
-      <c r="F18" s="117"/>
+      <c r="F18" s="122"/>
     </row>
     <row r="19" spans="1:6" ht="30">
       <c r="A19" s="94" t="str">
@@ -20431,7 +20445,7 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="116" t="str">
+      <c r="A22" s="121" t="str">
         <f>$A$19&amp;"/"&amp;$B$19</f>
         <v>emna-extraclase /emnaUsuariosMS</v>
       </c>
@@ -20450,12 +20464,12 @@
         <f>C21</f>
         <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/urls </v>
       </c>
-      <c r="F22" s="116" t="s">
+      <c r="F22" s="121" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="117"/>
+      <c r="A23" s="122"/>
       <c r="B23" s="96"/>
       <c r="C23" s="96"/>
       <c r="D23" s="96" t="str">
@@ -20463,7 +20477,7 @@
         <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/models </v>
       </c>
       <c r="E23" s="96"/>
-      <c r="F23" s="117"/>
+      <c r="F23" s="122"/>
     </row>
     <row r="24" spans="1:6" ht="30">
       <c r="A24" s="77" t="str">
@@ -20490,7 +20504,7 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="116" t="str">
+      <c r="A25" s="121" t="str">
         <f>$A$19&amp;"/"&amp;$B$19</f>
         <v>emna-extraclase /emnaUsuariosMS</v>
       </c>
@@ -20506,12 +20520,12 @@
         <f>C22</f>
         <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/views </v>
       </c>
-      <c r="F25" s="116" t="s">
+      <c r="F25" s="121" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="117"/>
+      <c r="A26" s="122"/>
       <c r="B26" s="96"/>
       <c r="C26" s="96"/>
       <c r="D26" s="96"/>
@@ -20519,7 +20533,7 @@
         <f>C24</f>
         <v xml:space="preserve">emna-extraclase /emnaUsuariosMS/serializers </v>
       </c>
-      <c r="F26" s="117"/>
+      <c r="F26" s="122"/>
     </row>
     <row r="27" spans="1:6" ht="30">
       <c r="A27" s="94" t="str">
@@ -20582,7 +20596,7 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="116" t="str">
+      <c r="A30" s="121" t="str">
         <f t="shared" si="1"/>
         <v>emna-extraclase /emnaSeguridadMS</v>
       </c>
@@ -20601,12 +20615,12 @@
         <f>C29</f>
         <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/urls </v>
       </c>
-      <c r="F30" s="116" t="s">
+      <c r="F30" s="121" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="117"/>
+      <c r="A31" s="122"/>
       <c r="B31" s="96"/>
       <c r="C31" s="96"/>
       <c r="D31" s="96" t="str">
@@ -20614,7 +20628,7 @@
         <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/models </v>
       </c>
       <c r="E31" s="96"/>
-      <c r="F31" s="117"/>
+      <c r="F31" s="122"/>
     </row>
     <row r="32" spans="1:6" ht="30">
       <c r="A32" s="77" t="str">
@@ -20641,7 +20655,7 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="116" t="str">
+      <c r="A33" s="121" t="str">
         <f t="shared" si="1"/>
         <v>emna-extraclase /emnaSeguridadMS</v>
       </c>
@@ -20657,12 +20671,12 @@
         <f>C30</f>
         <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/views </v>
       </c>
-      <c r="F33" s="116" t="s">
+      <c r="F33" s="121" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="117"/>
+      <c r="A34" s="122"/>
       <c r="B34" s="77"/>
       <c r="C34" s="77"/>
       <c r="D34" s="77"/>
@@ -20670,7 +20684,7 @@
         <f>C32</f>
         <v xml:space="preserve">emna-extraclase /emnaSeguridadMS/serializers </v>
       </c>
-      <c r="F34" s="117"/>
+      <c r="F34" s="122"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="94" t="str">
@@ -20692,13 +20706,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A26"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F30:F31"/>
@@ -20711,6 +20718,13 @@
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{94EFA083-0C5B-412C-8DD7-22C9E2BEB40A}"/>

</xml_diff>